<commit_message>
Update wiki data pipeline
</commit_message>
<xml_diff>
--- a/3-data/output/article-selection/mpox-linked-pages-classified.xlsx
+++ b/3-data/output/article-selection/mpox-linked-pages-classified.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/mpox-wiki-analysis/3-data/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/mpox-wiki-analysis/3-data/output/article-selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D2C32-8BFD-9C49-92F3-854152C7CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6875D8CC-70FE-704A-9833-00E42DBB523A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="172" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="172" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2121,7 +2121,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>